<commit_message>
Improved the data fact sheet create function and the criteria table
</commit_message>
<xml_diff>
--- a/App/data/CriteriaTable.xlsx
+++ b/App/data/CriteriaTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Work\TT_Backup2\WY_Tool\App_V2\data\Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Work\TT_Backup2\WY_Tool\2024_Region8_AssessmentTool\App\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC00F9A-A2E4-45B4-91BE-ED2D8BC96200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5262D87A-8DD1-49A0-8D3F-0130DF814CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{35CC37A3-810C-4E31-8A73-D55029217432}"/>
   </bookViews>
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4587" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4588" uniqueCount="215">
   <si>
     <t>State</t>
   </si>
@@ -1028,7 +1028,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1056,6 +1056,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1089,11 +1092,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1462,8 +1460,8 @@
   <dimension ref="A1:P150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H151" sqref="H151"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -2144,7 +2142,7 @@
       </c>
       <c r="P15" s="2"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2189,7 +2187,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -2277,7 +2275,7 @@
       </c>
       <c r="P18" s="2"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -2322,7 +2320,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -2539,7 +2537,7 @@
       </c>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -2584,7 +2582,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
@@ -3010,7 +3008,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
@@ -3055,7 +3053,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
@@ -3143,7 +3141,7 @@
       </c>
       <c r="P38" s="2"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>14</v>
       </c>
@@ -3188,7 +3186,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>14</v>
       </c>
@@ -3450,7 +3448,7 @@
       </c>
       <c r="P45" s="2"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -3495,7 +3493,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>14</v>
       </c>
@@ -4392,7 +4390,7 @@
       </c>
       <c r="P67" s="2"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A68" s="2" t="s">
         <v>14</v>
       </c>
@@ -4728,7 +4726,7 @@
       </c>
       <c r="P75" s="2"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A76" s="2" t="s">
         <v>14</v>
       </c>
@@ -4773,7 +4771,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
       <c r="A77" s="2" t="s">
         <v>14</v>
       </c>
@@ -4906,7 +4904,7 @@
       </c>
       <c r="P79" s="2"/>
     </row>
-    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A80" s="2" t="s">
         <v>88</v>
       </c>
@@ -4951,7 +4949,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A81" s="2" t="s">
         <v>88</v>
       </c>
@@ -4996,7 +4994,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A82" s="2" t="s">
         <v>88</v>
       </c>
@@ -5039,7 +5037,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A83" s="2" t="s">
         <v>88</v>
       </c>
@@ -5082,7 +5080,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A84" s="2" t="s">
         <v>88</v>
       </c>
@@ -5125,7 +5123,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A85" s="2" t="s">
         <v>88</v>
       </c>
@@ -5168,7 +5166,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A86" s="2" t="s">
         <v>88</v>
       </c>
@@ -5211,7 +5209,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A87" s="2" t="s">
         <v>88</v>
       </c>
@@ -5254,7 +5252,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:16" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A88" s="4" t="s">
         <v>88</v>
       </c>
@@ -5295,48 +5293,48 @@
       </c>
       <c r="P88" s="4"/>
     </row>
-    <row r="89" spans="1:16" s="36" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B89" s="36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C89" s="36" t="s">
+    <row r="89" spans="1:16" s="25" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A89" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C89" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D89" s="36" t="s">
+      <c r="D89" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="E89" s="36" t="s">
+      <c r="E89" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F89" s="36" t="s">
+      <c r="F89" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="H89" s="36">
+      <c r="H89" s="25">
         <v>5.6</v>
       </c>
-      <c r="I89" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="J89" s="37">
+      <c r="I89" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J89" s="26">
         <v>0.1</v>
       </c>
-      <c r="K89" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="L89" s="36">
-        <v>3</v>
-      </c>
-      <c r="M89" s="36">
-        <v>3</v>
-      </c>
-      <c r="O89" s="38">
+      <c r="K89" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="L89" s="25">
+        <v>3</v>
+      </c>
+      <c r="M89" s="25">
+        <v>3</v>
+      </c>
+      <c r="O89" s="27">
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A90" s="2" t="s">
         <v>88</v>
       </c>
@@ -5379,7 +5377,7 @@
       </c>
       <c r="P90" s="2"/>
     </row>
-    <row r="91" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A91" s="2" t="s">
         <v>88</v>
       </c>
@@ -5422,7 +5420,7 @@
       </c>
       <c r="P91" s="2"/>
     </row>
-    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A92" s="2" t="s">
         <v>88</v>
       </c>
@@ -5465,7 +5463,7 @@
       </c>
       <c r="P92" s="2"/>
     </row>
-    <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A93" s="2" t="s">
         <v>88</v>
       </c>
@@ -5508,7 +5506,7 @@
       </c>
       <c r="P93" s="2"/>
     </row>
-    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A94" s="2" t="s">
         <v>88</v>
       </c>
@@ -5641,7 +5639,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A97" s="2" t="s">
         <v>88</v>
       </c>
@@ -5684,7 +5682,7 @@
       </c>
       <c r="P97" s="2"/>
     </row>
-    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A98" s="2" t="s">
         <v>88</v>
       </c>
@@ -5727,7 +5725,7 @@
       </c>
       <c r="P98" s="2"/>
     </row>
-    <row r="99" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A99" s="2" t="s">
         <v>88</v>
       </c>
@@ -5770,37 +5768,39 @@
       </c>
       <c r="P99" s="2"/>
     </row>
-    <row r="100" spans="1:16" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A100" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="B100" s="39" t="s">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A100" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C100" s="39" t="s">
+      <c r="C100" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D100" s="39"/>
-      <c r="E100" s="39" t="s">
+      <c r="D100" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E100" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F100" s="39" t="s">
+      <c r="F100" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H100" s="39">
+      <c r="H100" s="2">
         <v>100</v>
       </c>
-      <c r="I100" s="39" t="s">
+      <c r="I100" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="L100" s="39">
-        <v>3</v>
-      </c>
-      <c r="M100" s="39">
-        <v>3</v>
-      </c>
-      <c r="N100" s="39"/>
-      <c r="O100" s="39">
+      <c r="L100" s="2">
+        <v>3</v>
+      </c>
+      <c r="M100" s="2">
+        <v>3</v>
+      </c>
+      <c r="N100" s="2"/>
+      <c r="O100" s="2">
         <v>2</v>
       </c>
     </row>
@@ -5984,7 +5984,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A105" s="2" t="s">
         <v>88</v>
       </c>
@@ -6027,7 +6027,7 @@
       </c>
       <c r="P105" s="2"/>
     </row>
-    <row r="106" spans="1:16" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A106" s="4" t="s">
         <v>88</v>
       </c>
@@ -6068,7 +6068,7 @@
       </c>
       <c r="P106" s="4"/>
     </row>
-    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A107" s="2" t="s">
         <v>88</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A108" s="2" t="s">
         <v>88</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A109" s="2" t="s">
         <v>88</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A110" s="2" t="s">
         <v>88</v>
       </c>
@@ -6238,7 +6238,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A111" s="2" t="s">
         <v>88</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="112" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A112" s="2" t="s">
         <v>88</v>
       </c>
@@ -6324,7 +6324,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="113" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A113" s="2" t="s">
         <v>88</v>
       </c>
@@ -6457,7 +6457,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="116" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A116" s="2" t="s">
         <v>88</v>
       </c>
@@ -6500,7 +6500,7 @@
       </c>
       <c r="P116" s="2"/>
     </row>
-    <row r="117" spans="1:16" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A117" s="4" t="s">
         <v>88</v>
       </c>
@@ -6541,7 +6541,7 @@
       </c>
       <c r="P117" s="4"/>
     </row>
-    <row r="118" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A118" s="2" t="s">
         <v>88</v>
       </c>
@@ -6584,7 +6584,7 @@
       </c>
       <c r="P118" s="2"/>
     </row>
-    <row r="119" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A119" s="2" t="s">
         <v>88</v>
       </c>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="P119" s="2"/>
     </row>
-    <row r="120" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A120" s="2" t="s">
         <v>88</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="123" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A123" s="2" t="s">
         <v>88</v>
       </c>
@@ -6803,7 +6803,7 @@
       </c>
       <c r="P123" s="2"/>
     </row>
-    <row r="124" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A124" s="2" t="s">
         <v>88</v>
       </c>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="P124" s="2"/>
     </row>
-    <row r="125" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A125" s="2" t="s">
         <v>88</v>
       </c>
@@ -6873,7 +6873,7 @@
       </c>
       <c r="P125" s="2"/>
     </row>
-    <row r="126" spans="1:16" s="2" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:16" s="2" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>88</v>
       </c>
@@ -6902,7 +6902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:16" s="2" customFormat="1" ht="13.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:16" s="2" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>88</v>
       </c>
@@ -6937,7 +6937,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="128" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A128" s="2" t="s">
         <v>88</v>
       </c>
@@ -6980,7 +6980,7 @@
       </c>
       <c r="P128" s="2"/>
     </row>
-    <row r="129" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A129" s="2" t="s">
         <v>88</v>
       </c>
@@ -7023,7 +7023,7 @@
       </c>
       <c r="P129" s="2"/>
     </row>
-    <row r="130" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A130" s="2" t="s">
         <v>88</v>
       </c>
@@ -7066,7 +7066,7 @@
       </c>
       <c r="P130" s="2"/>
     </row>
-    <row r="131" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A131" s="2" t="s">
         <v>88</v>
       </c>
@@ -7109,7 +7109,7 @@
       </c>
       <c r="P131" s="2"/>
     </row>
-    <row r="132" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A132" s="2" t="s">
         <v>88</v>
       </c>
@@ -7152,7 +7152,7 @@
       </c>
       <c r="P132" s="2"/>
     </row>
-    <row r="133" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A133" s="2" t="s">
         <v>88</v>
       </c>
@@ -7193,7 +7193,7 @@
       </c>
       <c r="P133" s="2"/>
     </row>
-    <row r="134" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A134" s="2" t="s">
         <v>88</v>
       </c>
@@ -7234,7 +7234,7 @@
       </c>
       <c r="P134" s="2"/>
     </row>
-    <row r="135" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A135" s="2" t="s">
         <v>88</v>
       </c>
@@ -7277,7 +7277,7 @@
       </c>
       <c r="P135" s="2"/>
     </row>
-    <row r="136" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A136" s="2" t="s">
         <v>88</v>
       </c>
@@ -7320,7 +7320,7 @@
       </c>
       <c r="P136" s="2"/>
     </row>
-    <row r="137" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A137" s="2" t="s">
         <v>88</v>
       </c>
@@ -7363,7 +7363,7 @@
       </c>
       <c r="P137" s="2"/>
     </row>
-    <row r="138" spans="1:16" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A138" s="4" t="s">
         <v>88</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="139" spans="1:16" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A139" s="4" t="s">
         <v>88</v>
       </c>
@@ -7445,7 +7445,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="140" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A140" s="2" t="s">
         <v>88</v>
       </c>
@@ -7488,7 +7488,7 @@
       </c>
       <c r="P140" s="2"/>
     </row>
-    <row r="141" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A141" s="2" t="s">
         <v>88</v>
       </c>
@@ -7531,7 +7531,7 @@
       </c>
       <c r="P141" s="2"/>
     </row>
-    <row r="142" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A142" s="2" t="s">
         <v>88</v>
       </c>
@@ -7619,7 +7619,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="144" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A144" s="2" t="s">
         <v>88</v>
       </c>
@@ -7662,7 +7662,7 @@
       </c>
       <c r="P144" s="2"/>
     </row>
-    <row r="145" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A145" s="2" t="s">
         <v>88</v>
       </c>
@@ -7705,7 +7705,7 @@
       </c>
       <c r="P145" s="2"/>
     </row>
-    <row r="146" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A146" s="2" t="s">
         <v>88</v>
       </c>
@@ -7748,7 +7748,7 @@
       </c>
       <c r="P146" s="2"/>
     </row>
-    <row r="147" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A147" s="2" t="s">
         <v>88</v>
       </c>
@@ -7881,7 +7881,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="150" spans="1:16" hidden="1" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A150" s="2" t="s">
         <v>88</v>
       </c>
@@ -7926,9 +7926,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:M150" xr:uid="{F829AA66-7AE2-4090-AC3D-2A3F7B1348C8}">
-    <filterColumn colId="12">
+    <filterColumn colId="1">
       <filters>
-        <filter val="1"/>
+        <filter val="MT"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -8888,7 +8888,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F95" sqref="F95"/>
+      <selection pane="bottomLeft" activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -12073,7 +12073,7 @@
       <c r="N86" t="s">
         <v>91</v>
       </c>
-      <c r="O86" s="29" t="s">
+      <c r="O86" s="32" t="s">
         <v>179</v>
       </c>
     </row>
@@ -12108,7 +12108,7 @@
       <c r="N87" t="s">
         <v>91</v>
       </c>
-      <c r="O87" s="29"/>
+      <c r="O87" s="32"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
@@ -12141,7 +12141,7 @@
       <c r="N88" t="s">
         <v>91</v>
       </c>
-      <c r="O88" s="29"/>
+      <c r="O88" s="32"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
@@ -12174,7 +12174,7 @@
       <c r="N89" t="s">
         <v>91</v>
       </c>
-      <c r="O89" s="29"/>
+      <c r="O89" s="32"/>
     </row>
     <row r="90" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A90" s="12" t="s">
@@ -12207,7 +12207,7 @@
       <c r="N90" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="O90" s="30" t="s">
+      <c r="O90" s="33" t="s">
         <v>181</v>
       </c>
     </row>
@@ -12242,7 +12242,7 @@
       <c r="N91" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="O91" s="30"/>
+      <c r="O91" s="33"/>
     </row>
     <row r="92" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
@@ -12765,7 +12765,7 @@
       <c r="L105">
         <v>3</v>
       </c>
-      <c r="O105" s="31" t="s">
+      <c r="O105" s="34" t="s">
         <v>186</v>
       </c>
     </row>
@@ -12806,7 +12806,7 @@
       <c r="L106">
         <v>3</v>
       </c>
-      <c r="O106" s="32"/>
+      <c r="O106" s="35"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
@@ -12851,7 +12851,7 @@
       <c r="N107" t="s">
         <v>95</v>
       </c>
-      <c r="O107" s="33"/>
+      <c r="O107" s="36"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
@@ -12896,7 +12896,7 @@
       <c r="N108" t="s">
         <v>95</v>
       </c>
-      <c r="O108" s="34"/>
+      <c r="O108" s="37"/>
     </row>
     <row r="109" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A109" s="8" t="s">
@@ -12947,7 +12947,7 @@
         <v>188</v>
       </c>
       <c r="H110" s="15"/>
-      <c r="O110" s="25" t="s">
+      <c r="O110" s="28" t="s">
         <v>189</v>
       </c>
     </row>
@@ -12965,7 +12965,7 @@
         <v>190</v>
       </c>
       <c r="H111" s="15"/>
-      <c r="O111" s="26"/>
+      <c r="O111" s="29"/>
     </row>
     <row r="112" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A112" s="14" t="s">
@@ -14032,7 +14032,7 @@
       <c r="H141" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="O141" s="25" t="s">
+      <c r="O141" s="28" t="s">
         <v>204</v>
       </c>
     </row>
@@ -14055,7 +14055,7 @@
       <c r="H142" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="O142" s="35"/>
+      <c r="O142" s="38"/>
     </row>
     <row r="143" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A143" s="17" t="s">
@@ -14076,7 +14076,7 @@
       <c r="H143" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="O143" s="26"/>
+      <c r="O143" s="29"/>
     </row>
     <row r="144" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A144" s="17" t="s">
@@ -14178,7 +14178,7 @@
         <v>188</v>
       </c>
       <c r="H147" s="16"/>
-      <c r="O147" s="25" t="s">
+      <c r="O147" s="28" t="s">
         <v>189</v>
       </c>
     </row>
@@ -14199,7 +14199,7 @@
         <v>190</v>
       </c>
       <c r="H148" s="16"/>
-      <c r="O148" s="26"/>
+      <c r="O148" s="29"/>
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
@@ -14618,7 +14618,7 @@
         <v>188</v>
       </c>
       <c r="H161" s="16"/>
-      <c r="O161" s="27" t="s">
+      <c r="O161" s="30" t="s">
         <v>189</v>
       </c>
     </row>
@@ -14639,7 +14639,7 @@
         <v>190</v>
       </c>
       <c r="H162" s="16"/>
-      <c r="O162" s="28"/>
+      <c r="O162" s="31"/>
     </row>
     <row r="163" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A163" s="1" t="s">
@@ -15367,7 +15367,7 @@
   <dimension ref="A1:N171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>

</xml_diff>